<commit_message>
Re-calculated (again-again-again) column and gutter sizes, and repositioned columns accordingly.
</commit_message>
<xml_diff>
--- a/Tabular data.xlsx
+++ b/Tabular data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik\dev\pocket-operator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A86A35-A33B-4E9D-90E5-C364268038E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B39FD8-9892-4E47-B603-61C0DB7EF0AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7C7CCA55-A621-4F59-B792-6320104E8327}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>70,40</t>
   </si>
@@ -129,6 +129,51 @@
   </si>
   <si>
     <t>Noise</t>
+  </si>
+  <si>
+    <t>Spacing</t>
+  </si>
+  <si>
+    <t>Number columns</t>
+  </si>
+  <si>
+    <t>Width of left and right margins</t>
+  </si>
+  <si>
+    <t>Width of middle gutters</t>
+  </si>
+  <si>
+    <t>Guide positions</t>
+  </si>
+  <si>
+    <t>Col 1, RHS</t>
+  </si>
+  <si>
+    <t>Col 2, LHS</t>
+  </si>
+  <si>
+    <t>Col 2, RHS</t>
+  </si>
+  <si>
+    <t>Col 3, LHS</t>
+  </si>
+  <si>
+    <t>Width of paper</t>
+  </si>
+  <si>
+    <t>Therefore, width of columns</t>
+  </si>
+  <si>
+    <t>Col 3, RHS</t>
+  </si>
+  <si>
+    <t>Col 4, LHS</t>
+  </si>
+  <si>
+    <t>Col 4, RHS</t>
+  </si>
+  <si>
+    <t>Col 1, LHS</t>
   </si>
 </sst>
 </file>
@@ -591,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544D9A6-F3E0-4AE0-9D95-088BEF732D2F}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,6 +910,129 @@
         <v>32</v>
       </c>
     </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <f xml:space="preserve"> (D18 - (2*D20) - (D19-1) * D21) / D19</f>
+        <v>44.825000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24">
+        <f>D20</f>
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <f>C24+D22</f>
+        <v>51.175000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <f>C25+D21</f>
+        <v>57.175000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <f>C26+D22</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <f>C27+D21</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29">
+        <f>C28+D22</f>
+        <v>152.82499999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30">
+        <f>C29+D21</f>
+        <v>158.82499999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31">
+        <f>C30+D22</f>
+        <v>203.64999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added sync modes, and moved content around
</commit_message>
<xml_diff>
--- a/Tabular data.xlsx
+++ b/Tabular data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik\dev\pocket-operator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B39FD8-9892-4E47-B603-61C0DB7EF0AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE8075-AEC3-4AF5-9804-AF649E4353D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7C7CCA55-A621-4F59-B792-6320104E8327}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>70,40</t>
   </si>
@@ -86,15 +86,6 @@
     <t>Aliasing</t>
   </si>
   <si>
-    <t>OD</t>
-  </si>
-  <si>
-    <t>Rep 4</t>
-  </si>
-  <si>
-    <t>Rep 2</t>
-  </si>
-  <si>
     <t>LP filter</t>
   </si>
   <si>
@@ -107,12 +98,6 @@
     <t>HP sweep</t>
   </si>
   <si>
-    <t>Dist lo</t>
-  </si>
-  <si>
-    <t>Dist hi</t>
-  </si>
-  <si>
     <t>Retrig</t>
   </si>
   <si>
@@ -174,13 +159,64 @@
   </si>
   <si>
     <t>Col 1, LHS</t>
+  </si>
+  <si>
+    <t>Overdrive</t>
+  </si>
+  <si>
+    <t>Repeat 4</t>
+  </si>
+  <si>
+    <t>Repeat 2</t>
+  </si>
+  <si>
+    <t>Distort hi</t>
+  </si>
+  <si>
+    <t>Distort lo</t>
+  </si>
+  <si>
+    <t>Sync modes</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>SY0</t>
+  </si>
+  <si>
+    <t>SY1</t>
+  </si>
+  <si>
+    <t>SY2</t>
+  </si>
+  <si>
+    <t>SY3</t>
+  </si>
+  <si>
+    <t>SY4</t>
+  </si>
+  <si>
+    <t>SY5</t>
+  </si>
+  <si>
+    <t>Stereo</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>Mono/Sync</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +231,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -204,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -213,84 +257,357 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color rgb="FFA3A3A3"/>
+        <color theme="0" tint="-0.14996795556505021"/>
       </left>
       <right style="medium">
-        <color rgb="FFA3A3A3"/>
+        <color theme="0" tint="-0.14996795556505021"/>
       </right>
       <top style="medium">
-        <color rgb="FFA3A3A3"/>
+        <color theme="0" tint="-0.14996795556505021"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFA3A3A3"/>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.1498764000366222"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14996795556505021"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </left>
       <right style="thin">
         <color theme="0"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14990691854609822"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.14990691854609822"/>
       </left>
       <right style="thin">
         <color theme="0"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
       </bottom>
       <diagonal/>
     </border>
@@ -298,30 +615,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,288 +1009,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544D9A6-F3E0-4AE0-9D95-088BEF732D2F}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.6640625" customWidth="1"/>
+    <col min="1" max="4" width="9.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="2.5546875" customWidth="1"/>
-    <col min="7" max="7" width="2.33203125" customWidth="1"/>
-    <col min="8" max="8" width="2.5546875" customWidth="1"/>
-    <col min="9" max="9" width="2.33203125" customWidth="1"/>
-    <col min="10" max="10" width="2.5546875" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" customWidth="1"/>
-    <col min="12" max="12" width="2.5546875" customWidth="1"/>
-    <col min="13" max="13" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="2.77734375" customWidth="1"/>
+    <col min="7" max="7" width="2" customWidth="1"/>
+    <col min="8" max="8" width="2.77734375" customWidth="1"/>
+    <col min="9" max="9" width="2" customWidth="1"/>
+    <col min="10" max="10" width="2.77734375" customWidth="1"/>
+    <col min="11" max="11" width="2" customWidth="1"/>
+    <col min="12" max="12" width="2.77734375" customWidth="1"/>
+    <col min="13" max="13" width="2" customWidth="1"/>
+    <col min="16" max="16" width="4.77734375" customWidth="1"/>
+    <col min="17" max="18" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="str">
+      <c r="F3" s="9" t="str">
         <f>_xlfn.CONCAT(LEFT(A3,2), ",")</f>
         <v>70,</v>
       </c>
-      <c r="G3" s="5" t="str">
+      <c r="G3" s="10" t="str">
         <f>RIGHT(A3,2)</f>
         <v>40</v>
       </c>
-      <c r="H3" s="4" t="str">
+      <c r="H3" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B3,2), ",")</f>
         <v>80,</v>
       </c>
-      <c r="I3" s="5" t="str">
+      <c r="I3" s="12" t="str">
         <f>RIGHT(B3,2)</f>
         <v>40</v>
       </c>
-      <c r="J3" s="4" t="str">
+      <c r="J3" s="13" t="str">
         <f>_xlfn.CONCAT(LEFT(C3,2), ",")</f>
         <v>90,</v>
       </c>
-      <c r="K3" s="5" t="str">
+      <c r="K3" s="14" t="str">
         <f>RIGHT(C3,2)</f>
         <v>50</v>
       </c>
-      <c r="L3" s="4" t="str">
+      <c r="L3" s="15" t="str">
         <f>_xlfn.CONCAT(LEFT(D3,2), ",")</f>
         <v>60,</v>
       </c>
-      <c r="M3" s="5" t="str">
+      <c r="M3" s="16" t="str">
         <f>RIGHT(D3,2)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="str">
+      <c r="F4" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(A4,2), ",")</f>
         <v>50,</v>
       </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" s="17" t="str">
         <f>RIGHT(A4,2)</f>
         <v xml:space="preserve"> 0</v>
       </c>
-      <c r="H4" s="4" t="str">
+      <c r="H4" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B4,2), ",")</f>
         <v>30,</v>
       </c>
-      <c r="I4" s="5" t="str">
+      <c r="I4" s="12" t="str">
         <f>RIGHT(B4,2)</f>
         <v>30</v>
       </c>
-      <c r="J4" s="4" t="str">
+      <c r="J4" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(C4,2), ",")</f>
         <v>60,</v>
       </c>
-      <c r="K4" s="5" t="str">
+      <c r="K4" s="19" t="str">
         <f>RIGHT(C4,2)</f>
         <v>70</v>
       </c>
-      <c r="L4" s="4" t="str">
+      <c r="L4" s="20" t="str">
         <f>_xlfn.CONCAT(LEFT(D4,2), ",")</f>
         <v>50,</v>
       </c>
-      <c r="M4" s="5" t="str">
+      <c r="M4" s="21" t="str">
         <f>RIGHT(D4,2)</f>
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="P4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="str">
+      <c r="F5" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(A5,2), ",")</f>
         <v>45,</v>
       </c>
-      <c r="G5" s="7" t="str">
+      <c r="G5" s="17" t="str">
         <f>RIGHT(A5,2)</f>
         <v>50</v>
       </c>
-      <c r="H5" s="6" t="str">
+      <c r="H5" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B5,2), ",")</f>
         <v>60,</v>
       </c>
-      <c r="I5" s="7" t="str">
+      <c r="I5" s="12" t="str">
         <f>RIGHT(B5,2)</f>
         <v>60</v>
       </c>
-      <c r="J5" s="6" t="str">
+      <c r="J5" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(C5,2), ",")</f>
         <v>70,</v>
       </c>
-      <c r="K5" s="7" t="str">
+      <c r="K5" s="19" t="str">
         <f>RIGHT(C5,2)</f>
         <v>80</v>
       </c>
-      <c r="L5" s="6" t="str">
+      <c r="L5" s="20" t="str">
         <f>_xlfn.CONCAT(LEFT(D5,2), ",")</f>
         <v>55,</v>
       </c>
-      <c r="M5" s="7" t="str">
+      <c r="M5" s="21" t="str">
         <f>RIGHT(D5,2)</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="P5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="6" t="str">
+      <c r="F6" s="22" t="str">
         <f>_xlfn.CONCAT(LEFT(A6,2), ",")</f>
         <v>60,</v>
       </c>
-      <c r="G6" s="7" t="str">
+      <c r="G6" s="23" t="str">
         <f>RIGHT(A6,2)</f>
         <v>80</v>
       </c>
-      <c r="H6" s="6" t="str">
+      <c r="H6" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B6,2), ",")</f>
         <v>55,</v>
       </c>
-      <c r="I6" s="7" t="str">
+      <c r="I6" s="12" t="str">
         <f>RIGHT(B6,2)</f>
         <v>80</v>
       </c>
-      <c r="J6" s="6" t="str">
+      <c r="J6" s="24" t="str">
         <f>_xlfn.CONCAT(LEFT(C6,2), ",")</f>
         <v>65,</v>
       </c>
-      <c r="K6" s="7" t="str">
+      <c r="K6" s="25" t="str">
         <f>RIGHT(C6,2)</f>
         <v>30</v>
       </c>
-      <c r="L6" s="6" t="str">
+      <c r="L6" s="26" t="str">
         <f>_xlfn.CONCAT(LEFT(D6,2), ",")</f>
         <v>10,</v>
       </c>
-      <c r="M6" s="7" t="str">
+      <c r="M6" s="27" t="str">
         <f>RIGHT(D6,2)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="P6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="P8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="P9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="B12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="C12" s="28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="D12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="8" t="s">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="8" t="s">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="B14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D14" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="8" t="s">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>210</v>
@@ -925,7 +1366,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -933,7 +1374,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D20">
         <v>6.35</v>
@@ -941,7 +1382,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -949,7 +1390,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <f xml:space="preserve"> (D18 - (2*D20) - (D19-1) * D21) / D19</f>
@@ -958,12 +1399,12 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <f>D20</f>
@@ -972,7 +1413,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <f>C24+D22</f>
@@ -981,7 +1422,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <f>C25+D21</f>
@@ -990,7 +1431,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <f>C26+D22</f>
@@ -999,7 +1440,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <f>C27+D21</f>
@@ -1008,7 +1449,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C29">
         <f>C28+D22</f>
@@ -1017,7 +1458,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C30">
         <f>C29+D21</f>
@@ -1026,7 +1467,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C31">
         <f>C30+D22</f>

</xml_diff>

<commit_message>
Corrected default sound parameters; showed which effects are affect live playing.
</commit_message>
<xml_diff>
--- a/Tabular data.xlsx
+++ b/Tabular data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik\dev\pocket-operator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE8075-AEC3-4AF5-9804-AF649E4353D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72370411-F310-4CE2-861C-FC30BCAEB1DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7C7CCA55-A621-4F59-B792-6320104E8327}"/>
   </bookViews>
@@ -30,37 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
-  <si>
-    <t>70,40</t>
-  </si>
-  <si>
-    <t>80,40</t>
-  </si>
-  <si>
-    <t>90,50</t>
-  </si>
-  <si>
-    <t>60,10</t>
-  </si>
-  <si>
-    <t>30,30</t>
-  </si>
-  <si>
-    <t>60,70</t>
-  </si>
-  <si>
-    <t>50,70</t>
-  </si>
-  <si>
-    <t>45,50</t>
-  </si>
-  <si>
-    <t>60,60</t>
-  </si>
-  <si>
-    <t>70,80</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
   <si>
     <t>55,80</t>
   </si>
@@ -68,15 +38,6 @@
     <t>60,80</t>
   </si>
   <si>
-    <t>50, 0</t>
-  </si>
-  <si>
-    <t>10,30</t>
-  </si>
-  <si>
-    <t>65,30</t>
-  </si>
-  <si>
     <t>Default sound parameters</t>
   </si>
   <si>
@@ -210,6 +171,27 @@
   </si>
   <si>
     <t>Mono/Sync</t>
+  </si>
+  <si>
+    <t>52,80</t>
+  </si>
+  <si>
+    <t>52,76</t>
+  </si>
+  <si>
+    <t>52,20</t>
+  </si>
+  <si>
+    <t>51,75</t>
+  </si>
+  <si>
+    <t>52,75</t>
+  </si>
+  <si>
+    <t>51,80</t>
+  </si>
+  <si>
+    <t>50,80</t>
   </si>
 </sst>
 </file>
@@ -240,13 +222,19 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -615,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -695,6 +683,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,192 +1022,192 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="P1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="F3" s="9" t="str">
         <f>_xlfn.CONCAT(LEFT(A3,2), ",")</f>
-        <v>70,</v>
+        <v>60,</v>
       </c>
       <c r="G3" s="10" t="str">
         <f>RIGHT(A3,2)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H3" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B3,2), ",")</f>
-        <v>80,</v>
+        <v>55,</v>
       </c>
       <c r="I3" s="12" t="str">
         <f>RIGHT(B3,2)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J3" s="13" t="str">
         <f>_xlfn.CONCAT(LEFT(C3,2), ",")</f>
-        <v>90,</v>
+        <v>55,</v>
       </c>
       <c r="K3" s="14" t="str">
         <f>RIGHT(C3,2)</f>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="L3" s="15" t="str">
         <f>_xlfn.CONCAT(LEFT(D3,2), ",")</f>
-        <v>60,</v>
+        <v>52,</v>
       </c>
       <c r="M3" s="16" t="str">
         <f>RIGHT(D3,2)</f>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="F4" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(A4,2), ",")</f>
-        <v>50,</v>
+        <v>52,</v>
       </c>
       <c r="G4" s="17" t="str">
         <f>RIGHT(A4,2)</f>
-        <v xml:space="preserve"> 0</v>
+        <v>80</v>
       </c>
       <c r="H4" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B4,2), ",")</f>
-        <v>30,</v>
+        <v>52,</v>
       </c>
       <c r="I4" s="12" t="str">
         <f>RIGHT(B4,2)</f>
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="J4" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(C4,2), ",")</f>
-        <v>60,</v>
+        <v>52,</v>
       </c>
       <c r="K4" s="19" t="str">
         <f>RIGHT(C4,2)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="L4" s="20" t="str">
         <f>_xlfn.CONCAT(LEFT(D4,2), ",")</f>
-        <v>50,</v>
+        <v>52,</v>
       </c>
       <c r="M4" s="21" t="str">
         <f>RIGHT(D4,2)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F5" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(A5,2), ",")</f>
-        <v>45,</v>
+        <v>52,</v>
       </c>
       <c r="G5" s="17" t="str">
         <f>RIGHT(A5,2)</f>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H5" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B5,2), ",")</f>
-        <v>60,</v>
+        <v>51,</v>
       </c>
       <c r="I5" s="12" t="str">
         <f>RIGHT(B5,2)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="J5" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(C5,2), ",")</f>
-        <v>70,</v>
+        <v>51,</v>
       </c>
       <c r="K5" s="19" t="str">
         <f>RIGHT(C5,2)</f>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L5" s="20" t="str">
         <f>_xlfn.CONCAT(LEFT(D5,2), ",")</f>
-        <v>55,</v>
+        <v>52,</v>
       </c>
       <c r="M5" s="21" t="str">
         <f>RIGHT(D5,2)</f>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="F6" s="22" t="str">
         <f>_xlfn.CONCAT(LEFT(A6,2), ",")</f>
-        <v>60,</v>
+        <v>51,</v>
       </c>
       <c r="G6" s="23" t="str">
         <f>RIGHT(A6,2)</f>
@@ -1226,7 +1215,7 @@
       </c>
       <c r="H6" s="11" t="str">
         <f>_xlfn.CONCAT(LEFT(B6,2), ",")</f>
-        <v>55,</v>
+        <v>51,</v>
       </c>
       <c r="I6" s="12" t="str">
         <f>RIGHT(B6,2)</f>
@@ -1234,131 +1223,131 @@
       </c>
       <c r="J6" s="24" t="str">
         <f>_xlfn.CONCAT(LEFT(C6,2), ",")</f>
-        <v>65,</v>
+        <v>50,</v>
       </c>
       <c r="K6" s="25" t="str">
         <f>RIGHT(C6,2)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="L6" s="26" t="str">
         <f>_xlfn.CONCAT(LEFT(D6,2), ",")</f>
-        <v>10,</v>
+        <v>51,</v>
       </c>
       <c r="M6" s="27" t="str">
         <f>RIGHT(D6,2)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P7" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="P8" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>43</v>
+      <c r="A11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>21</v>
+      <c r="A12" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>46</v>
+      <c r="A13" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <v>210</v>
@@ -1366,7 +1355,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1374,7 +1363,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <v>6.35</v>
@@ -1382,7 +1371,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -1390,7 +1379,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <f xml:space="preserve"> (D18 - (2*D20) - (D19-1) * D21) / D19</f>
@@ -1399,12 +1388,12 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <f>D20</f>
@@ -1413,7 +1402,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C25">
         <f>C24+D22</f>
@@ -1422,7 +1411,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <f>C25+D21</f>
@@ -1431,7 +1420,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <f>C26+D22</f>
@@ -1440,7 +1429,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <f>C27+D21</f>
@@ -1449,7 +1438,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <f>C28+D22</f>
@@ -1458,7 +1447,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <f>C29+D21</f>
@@ -1467,7 +1456,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C31">
         <f>C30+D22</f>

</xml_diff>

<commit_message>
Corrected margins - yet again - and this time it does fold properly.
</commit_message>
<xml_diff>
--- a/Tabular data.xlsx
+++ b/Tabular data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik\dev\pocket-operator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72370411-F310-4CE2-861C-FC30BCAEB1DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAEA57E-E5FC-4A25-973F-CCFB4D48184F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7C7CCA55-A621-4F59-B792-6320104E8327}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>55,80</t>
   </si>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544D9A6-F3E0-4AE0-9D95-088BEF732D2F}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1405,8 +1405,8 @@
         <v>20</v>
       </c>
       <c r="C25">
-        <f>C24+D22</f>
-        <v>51.175000000000004</v>
+        <f>D18/D19-D21/2</f>
+        <v>49.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1414,8 +1414,8 @@
         <v>21</v>
       </c>
       <c r="C26">
-        <f>C25+D21</f>
-        <v>57.175000000000004</v>
+        <f>D18/D19+D21/2</f>
+        <v>55.5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1423,7 +1423,7 @@
         <v>22</v>
       </c>
       <c r="C27">
-        <f>C26+D22</f>
+        <f>D18/2-D21/2</f>
         <v>102</v>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
         <v>23</v>
       </c>
       <c r="C28">
-        <f>C27+D21</f>
+        <f>D18/2+D21/2</f>
         <v>108</v>
       </c>
     </row>
@@ -1441,8 +1441,8 @@
         <v>26</v>
       </c>
       <c r="C29">
-        <f>C28+D22</f>
-        <v>152.82499999999999</v>
+        <f>D18/D19*3-D21/2</f>
+        <v>154.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1450,8 +1450,8 @@
         <v>27</v>
       </c>
       <c r="C30">
-        <f>C29+D21</f>
-        <v>158.82499999999999</v>
+        <f>D18/D19*3+D21/2</f>
+        <v>160.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1459,8 +1459,8 @@
         <v>28</v>
       </c>
       <c r="C31">
-        <f>C30+D22</f>
-        <v>203.64999999999998</v>
+        <f>D18-D20</f>
+        <v>203.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Darker grey for effects that work during live play
</commit_message>
<xml_diff>
--- a/Tabular data.xlsx
+++ b/Tabular data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik\dev\pocket-operator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAEA57E-E5FC-4A25-973F-CCFB4D48184F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45840D9F-A8EF-4FEF-B66A-7D548E24E607}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7C7CCA55-A621-4F59-B792-6320104E8327}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
   <si>
     <t>55,80</t>
   </si>
@@ -231,7 +231,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544D9A6-F3E0-4AE0-9D95-088BEF732D2F}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D14" sqref="A11:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>